<commit_message>
only problems when units in the HTML are not the same as in the xlsx
</commit_message>
<xml_diff>
--- a/Lista_de_productos.xlsx
+++ b/Lista_de_productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\110414\PycharmProjects\Seguidor-de-precios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7061FFA-E614-4CBA-B8B2-83E70905A1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447F61ED-5073-4488-AD80-12BDE132CD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-9300" yWindow="4245" windowWidth="17280" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" r:id="rId1"/>
@@ -475,9 +475,6 @@
     <t>https://supermercado.eroski.es/es/productdetail/23777527-picada-mixta-de-vacuno-cerdo-bikain-bandeja-500-g/</t>
   </si>
   <si>
-    <t>https://supermercado.eroski.es/es/productdetail/22621643-huevo-fresco-suelo-xl-hobea-carton-12-uds/</t>
-  </si>
-  <si>
     <t>HUEVOS XL</t>
   </si>
   <si>
@@ -595,9 +592,6 @@
     <t xml:space="preserve">GULAS </t>
   </si>
   <si>
-    <t xml:space="preserve">PRODUCTOS </t>
-  </si>
-  <si>
     <t>https://supermercado.eroski.es/es/productdetail/226175-merluza-entera-pieza-al-peso-aprox-15-kg/</t>
   </si>
   <si>
@@ -820,9 +814,6 @@
     <t>https://www.online.bmsupermercados.es/es/p/abrillantador-lavavajillas-500-ml/75017</t>
   </si>
   <si>
-    <t>https://www.online.bmsupermercados.es/es/p/aceite-de-girasol-1-l/1381</t>
-  </si>
-  <si>
     <t>https://www.online.bmsupermercados.es/es/p/aceite-de-oliva-suave-1-l/5475</t>
   </si>
   <si>
@@ -1118,6 +1109,15 @@
   </si>
   <si>
     <t>MENSAJE</t>
+  </si>
+  <si>
+    <t>https://supermercado.eroski.es/es/productdetail/17081696-huevo-fresco-xl-pais-vasco-eroski-carton-12-uds/</t>
+  </si>
+  <si>
+    <t>PRODUCTOS</t>
+  </si>
+  <si>
+    <t>https://www.online.bmsupermercados.es/es/p/aceite-de-girasol-1-l/1011</t>
   </si>
 </sst>
 </file>
@@ -1690,9 +1690,9 @@
   </sheetPr>
   <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G92" sqref="G92:G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1700,7 +1700,7 @@
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" style="25" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="25" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" customWidth="1"/>
     <col min="6" max="6" width="123" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="84.6640625" customWidth="1"/>
@@ -1709,16 +1709,16 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>185</v>
+        <v>358</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>79</v>
@@ -1727,7 +1727,7 @@
         <v>80</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>81</v>
@@ -1741,7 +1741,7 @@
         <v>48</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D2" s="27" t="str">
         <f>VLOOKUP(C2,TablaUnidades[#All],2,FALSE)</f>
@@ -1749,10 +1749,10 @@
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -1764,18 +1764,18 @@
         <v>1</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D3" s="27" t="str">
         <f>VLOOKUP(C3,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por litro</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>260</v>
+      <c r="G3" s="12" t="s">
+        <v>359</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1787,7 +1787,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D4" s="27" t="str">
         <f>VLOOKUP(C4,TablaUnidades[#All],2,FALSE)</f>
@@ -1797,8 +1797,8 @@
       <c r="F4" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>261</v>
+      <c r="G4" s="12" t="s">
+        <v>258</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -1810,7 +1810,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D5" s="27" t="str">
         <f>VLOOKUP(C5,TablaUnidades[#All],2,FALSE)</f>
@@ -1821,7 +1821,7 @@
         <v>88</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -1833,7 +1833,7 @@
         <v>31</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D6" s="27" t="str">
         <f>VLOOKUP(C6,TablaUnidades[#All],2,FALSE)</f>
@@ -1844,7 +1844,7 @@
         <v>87</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -1853,10 +1853,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D7" s="27" t="str">
         <f>VLOOKUP(C7,TablaUnidades[#All],2,FALSE)</f>
@@ -1864,10 +1864,10 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -1879,7 +1879,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D8" s="27" t="str">
         <f>VLOOKUP(C8,TablaUnidades[#All],2,FALSE)</f>
@@ -1887,10 +1887,10 @@
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -1902,7 +1902,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D9" s="27" t="str">
         <f>VLOOKUP(C9,TablaUnidades[#All],2,FALSE)</f>
@@ -1913,7 +1913,7 @@
         <v>96</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -1925,7 +1925,7 @@
         <v>32</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D10" s="27" t="str">
         <f>VLOOKUP(C10,TablaUnidades[#All],2,FALSE)</f>
@@ -1936,7 +1936,7 @@
         <v>106</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -1948,7 +1948,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D11" s="27" t="str">
         <f>VLOOKUP(C11,TablaUnidades[#All],2,FALSE)</f>
@@ -1959,7 +1959,7 @@
         <v>121</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -1968,10 +1968,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D12" s="27" t="str">
         <f>VLOOKUP(C12,TablaUnidades[#All],2,FALSE)</f>
@@ -1979,10 +1979,10 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -1994,7 +1994,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D13" s="27" t="str">
         <f>VLOOKUP(C13,TablaUnidades[#All],2,FALSE)</f>
@@ -2002,10 +2002,10 @@
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -2014,10 +2014,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D14" s="27" t="str">
         <f>VLOOKUP(C14,TablaUnidades[#All],2,FALSE)</f>
@@ -2025,10 +2025,10 @@
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -2040,7 +2040,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D15" s="27" t="str">
         <f>VLOOKUP(C15,TablaUnidades[#All],2,FALSE)</f>
@@ -2051,7 +2051,7 @@
         <v>113</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -2063,7 +2063,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D16" s="27" t="str">
         <f>VLOOKUP(C16,TablaUnidades[#All],2,FALSE)</f>
@@ -2074,7 +2074,7 @@
         <v>93</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -2086,7 +2086,7 @@
         <v>35</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D17" s="27" t="str">
         <f>VLOOKUP(C17,TablaUnidades[#All],2,FALSE)</f>
@@ -2097,7 +2097,7 @@
         <v>107</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -2109,7 +2109,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D18" s="27" t="str">
         <f>VLOOKUP(C18,TablaUnidades[#All],2,FALSE)</f>
@@ -2117,10 +2117,10 @@
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -2129,10 +2129,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D19" s="27" t="str">
         <f>VLOOKUP(C19,TablaUnidades[#All],2,FALSE)</f>
@@ -2140,10 +2140,10 @@
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -2152,10 +2152,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D20" s="27" t="str">
         <f>VLOOKUP(C20,TablaUnidades[#All],2,FALSE)</f>
@@ -2163,10 +2163,10 @@
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H20" s="1"/>
     </row>
@@ -2175,7 +2175,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="27" t="e">
@@ -2195,7 +2195,7 @@
         <v>67</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D22" s="27" t="str">
         <f>VLOOKUP(C22,TablaUnidades[#All],2,FALSE)</f>
@@ -2203,10 +2203,10 @@
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H22" s="1"/>
     </row>
@@ -2218,7 +2218,7 @@
         <v>63</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D23" s="27" t="str">
         <f>VLOOKUP(C23,TablaUnidades[#All],2,FALSE)</f>
@@ -2226,10 +2226,10 @@
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H23" s="1"/>
     </row>
@@ -2241,7 +2241,7 @@
         <v>33</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D24" s="27" t="str">
         <f>VLOOKUP(C24,TablaUnidades[#All],2,FALSE)</f>
@@ -2252,7 +2252,7 @@
         <v>108</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H24" s="1"/>
     </row>
@@ -2261,10 +2261,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D25" s="27" t="str">
         <f>VLOOKUP(C25,TablaUnidades[#All],2,FALSE)</f>
@@ -2272,10 +2272,10 @@
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -2284,10 +2284,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D26" s="27" t="str">
         <f>VLOOKUP(C26,TablaUnidades[#All],2,FALSE)</f>
@@ -2295,10 +2295,10 @@
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H26" s="1"/>
     </row>
@@ -2307,10 +2307,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D27" s="27" t="str">
         <f>VLOOKUP(C27,TablaUnidades[#All],2,FALSE)</f>
@@ -2318,7 +2318,7 @@
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2331,7 +2331,7 @@
         <v>38</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D28" s="27" t="str">
         <f>VLOOKUP(C28,TablaUnidades[#All],2,FALSE)</f>
@@ -2342,7 +2342,7 @@
         <v>134</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H28" s="1"/>
     </row>
@@ -2354,7 +2354,7 @@
         <v>64</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D29" s="27" t="str">
         <f>VLOOKUP(C29,TablaUnidades[#All],2,FALSE)</f>
@@ -2362,33 +2362,33 @@
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D30" s="27" t="str">
         <f>VLOOKUP(C30,TablaUnidades[#All],2,FALSE)</f>
         <v>Comprueba que el manojo en todos los supers es del mismo tamaño (3 unidades cada manojo, por ejemplo)</v>
       </c>
       <c r="E30" s="6"/>
-      <c r="F30" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>284</v>
+      <c r="F30" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="H30" s="1"/>
     </row>
@@ -2397,7 +2397,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C31" s="22"/>
       <c r="D31" s="27" t="e">
@@ -2414,10 +2414,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D32" s="27" t="str">
         <f>VLOOKUP(C32,TablaUnidades[#All],2,FALSE)</f>
@@ -2425,10 +2425,10 @@
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H32" s="1"/>
     </row>
@@ -2437,10 +2437,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D33" s="27" t="str">
         <f>VLOOKUP(C33,TablaUnidades[#All],2,FALSE)</f>
@@ -2448,10 +2448,10 @@
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H33" s="1"/>
     </row>
@@ -2463,7 +2463,7 @@
         <v>22</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D34" s="27" t="str">
         <f>VLOOKUP(C34,TablaUnidades[#All],2,FALSE)</f>
@@ -2474,7 +2474,7 @@
         <v>102</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H34" s="1"/>
     </row>
@@ -2483,10 +2483,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D35" s="27" t="str">
         <f>VLOOKUP(C35,TablaUnidades[#All],2,FALSE)</f>
@@ -2494,10 +2494,10 @@
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="H35" s="1"/>
     </row>
@@ -2506,7 +2506,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C36" s="22"/>
       <c r="D36" s="27" t="e">
@@ -2526,7 +2526,7 @@
         <v>59</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D37" s="27" t="str">
         <f>VLOOKUP(C37,TablaUnidades[#All],2,FALSE)</f>
@@ -2534,10 +2534,10 @@
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="H37" s="1"/>
     </row>
@@ -2549,18 +2549,18 @@
         <v>61</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D38" s="27" t="str">
         <f>VLOOKUP(C38,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por unidad</v>
       </c>
       <c r="E38" s="6"/>
-      <c r="F38" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>290</v>
+      <c r="F38" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>287</v>
       </c>
       <c r="H38" s="1"/>
     </row>
@@ -2586,10 +2586,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D40" s="27" t="str">
         <f>VLOOKUP(C40,TablaUnidades[#All],2,FALSE)</f>
@@ -2597,10 +2597,10 @@
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="12" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H40" s="1"/>
     </row>
@@ -2609,10 +2609,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D41" s="27" t="str">
         <f>VLOOKUP(C41,TablaUnidades[#All],2,FALSE)</f>
@@ -2620,10 +2620,10 @@
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H41" s="1"/>
     </row>
@@ -2632,21 +2632,21 @@
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D42" s="27" t="str">
         <f>VLOOKUP(C42,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por dosis</v>
       </c>
       <c r="E42" s="6"/>
-      <c r="F42" s="1" t="s">
-        <v>234</v>
+      <c r="F42" s="12" t="s">
+        <v>232</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="H42" s="1"/>
     </row>
@@ -2658,7 +2658,7 @@
         <v>77</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D43" s="27" t="str">
         <f>VLOOKUP(C43,TablaUnidades[#All],2,FALSE)</f>
@@ -2666,10 +2666,10 @@
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="H43" s="1"/>
     </row>
@@ -2681,7 +2681,7 @@
         <v>137</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D44" s="27" t="str">
         <f>VLOOKUP(C44,TablaUnidades[#All],2,FALSE)</f>
@@ -2692,7 +2692,7 @@
         <v>136</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -2704,7 +2704,7 @@
         <v>29</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D45" s="27" t="str">
         <f>VLOOKUP(C45,TablaUnidades[#All],2,FALSE)</f>
@@ -2715,7 +2715,7 @@
         <v>116</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H45" s="1"/>
     </row>
@@ -2727,7 +2727,7 @@
         <v>18</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D46" s="27" t="str">
         <f>VLOOKUP(C46,TablaUnidades[#All],2,FALSE)</f>
@@ -2738,7 +2738,7 @@
         <v>99</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -2747,7 +2747,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C47" s="22"/>
       <c r="D47" s="27" t="e">
@@ -2767,7 +2767,7 @@
         <v>71</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D48" s="27" t="str">
         <f>VLOOKUP(C48,TablaUnidades[#All],2,FALSE)</f>
@@ -2775,10 +2775,10 @@
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H48" s="1"/>
     </row>
@@ -2787,10 +2787,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D49" s="27" t="str">
         <f>VLOOKUP(C49,TablaUnidades[#All],2,FALSE)</f>
@@ -2798,10 +2798,10 @@
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H49" s="1"/>
     </row>
@@ -2813,7 +2813,7 @@
         <v>9</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D50" s="27" t="str">
         <f>VLOOKUP(C50,TablaUnidades[#All],2,FALSE)</f>
@@ -2824,7 +2824,7 @@
         <v>119</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H50" s="1"/>
     </row>
@@ -2853,7 +2853,7 @@
         <v>90</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D52" s="27" t="str">
         <f>VLOOKUP(C52,TablaUnidades[#All],2,FALSE)</f>
@@ -2864,7 +2864,7 @@
         <v>89</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H52" s="1"/>
     </row>
@@ -2876,7 +2876,7 @@
         <v>26</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D53" s="27" t="str">
         <f>VLOOKUP(C53,TablaUnidades[#All],2,FALSE)</f>
@@ -2887,7 +2887,7 @@
         <v>98</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H53" s="1"/>
     </row>
@@ -2896,10 +2896,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D54" s="27" t="str">
         <f>VLOOKUP(C54,TablaUnidades[#All],2,FALSE)</f>
@@ -2907,10 +2907,10 @@
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H54" s="1"/>
     </row>
@@ -2922,7 +2922,7 @@
         <v>39</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D55" s="27" t="str">
         <f>VLOOKUP(C55,TablaUnidades[#All],2,FALSE)</f>
@@ -2933,7 +2933,7 @@
         <v>135</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H55" s="1"/>
     </row>
@@ -2945,7 +2945,7 @@
         <v>40</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D56" s="27" t="str">
         <f>VLOOKUP(C56,TablaUnidades[#All],2,FALSE)</f>
@@ -2956,7 +2956,7 @@
         <v>144</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H56" s="1"/>
     </row>
@@ -2968,7 +2968,7 @@
         <v>27</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D57" s="27" t="str">
         <f>VLOOKUP(C57,TablaUnidades[#All],2,FALSE)</f>
@@ -2979,7 +2979,7 @@
         <v>86</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H57" s="1"/>
     </row>
@@ -2988,21 +2988,21 @@
         <v>57</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D58" s="27" t="str">
         <f>VLOOKUP(C58,TablaUnidades[#All],2,FALSE)</f>
-        <v>precio por unidad</v>
+        <v>precio por docena</v>
       </c>
       <c r="E58" s="6"/>
       <c r="F58" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H58" s="1"/>
     </row>
@@ -3011,10 +3011,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D59" s="27" t="str">
         <f>VLOOKUP(C59,TablaUnidades[#All],2,FALSE)</f>
@@ -3022,10 +3022,10 @@
       </c>
       <c r="E59" s="6"/>
       <c r="F59" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H59" s="1"/>
     </row>
@@ -3034,21 +3034,21 @@
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D60" s="27" t="str">
         <f>VLOOKUP(C60,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por docena</v>
       </c>
       <c r="E60" s="6"/>
-      <c r="F60" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>309</v>
+      <c r="F60" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>306</v>
       </c>
       <c r="H60" s="1"/>
     </row>
@@ -3060,7 +3060,7 @@
         <v>43</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D61" s="27" t="str">
         <f>VLOOKUP(C61,TablaUnidades[#All],2,FALSE)</f>
@@ -3071,7 +3071,7 @@
         <v>138</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="H61" s="1"/>
     </row>
@@ -3083,7 +3083,7 @@
         <v>19</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D62" s="27" t="str">
         <f>VLOOKUP(C62,TablaUnidades[#All],2,FALSE)</f>
@@ -3091,10 +3091,10 @@
       </c>
       <c r="E62" s="6"/>
       <c r="F62" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="H62" s="1"/>
     </row>
@@ -3106,7 +3106,7 @@
         <v>3</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D63" s="27" t="str">
         <f>VLOOKUP(C63,TablaUnidades[#All],2,FALSE)</f>
@@ -3117,7 +3117,7 @@
         <v>127</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="H63" s="1"/>
     </row>
@@ -3129,7 +3129,7 @@
         <v>55</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D64" s="27" t="str">
         <f>VLOOKUP(C64,TablaUnidades[#All],2,FALSE)</f>
@@ -3137,10 +3137,10 @@
       </c>
       <c r="E64" s="6"/>
       <c r="F64" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H64" s="1"/>
     </row>
@@ -3149,10 +3149,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D65" s="27" t="str">
         <f>VLOOKUP(C65,TablaUnidades[#All],2,FALSE)</f>
@@ -3160,10 +3160,10 @@
       </c>
       <c r="E65" s="6"/>
       <c r="F65" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H65" s="1"/>
     </row>
@@ -3172,10 +3172,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D66" s="27" t="str">
         <f>VLOOKUP(C66,TablaUnidades[#All],2,FALSE)</f>
@@ -3183,10 +3183,10 @@
       </c>
       <c r="E66" s="6"/>
       <c r="F66" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H66" s="1"/>
     </row>
@@ -3198,7 +3198,7 @@
         <v>49</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D67" s="27" t="str">
         <f>VLOOKUP(C67,TablaUnidades[#All],2,FALSE)</f>
@@ -3206,10 +3206,10 @@
       </c>
       <c r="E67" s="6"/>
       <c r="F67" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="H67" s="1"/>
     </row>
@@ -3221,7 +3221,7 @@
         <v>111</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D68" s="27" t="str">
         <f>VLOOKUP(C68,TablaUnidades[#All],2,FALSE)</f>
@@ -3232,7 +3232,7 @@
         <v>110</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="H68" s="1"/>
     </row>
@@ -3244,7 +3244,7 @@
         <v>68</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D69" s="27" t="str">
         <f>VLOOKUP(C69,TablaUnidades[#All],2,FALSE)</f>
@@ -3255,7 +3255,7 @@
         <v>112</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H69" s="1"/>
     </row>
@@ -3264,10 +3264,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D70" s="27" t="str">
         <f>VLOOKUP(C70,TablaUnidades[#All],2,FALSE)</f>
@@ -3275,10 +3275,10 @@
       </c>
       <c r="E70" s="6"/>
       <c r="F70" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H70" s="1"/>
     </row>
@@ -3287,10 +3287,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D71" s="27" t="str">
         <f>VLOOKUP(C71,TablaUnidades[#All],2,FALSE)</f>
@@ -3298,10 +3298,10 @@
       </c>
       <c r="E71" s="6"/>
       <c r="F71" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H71" s="1"/>
     </row>
@@ -3313,7 +3313,7 @@
         <v>11</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D72" s="27" t="str">
         <f>VLOOKUP(C72,TablaUnidades[#All],2,FALSE)</f>
@@ -3324,7 +3324,7 @@
         <v>118</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="H72" s="1"/>
     </row>
@@ -3333,10 +3333,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C73" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D73" s="27" t="str">
         <f>VLOOKUP(C73,TablaUnidades[#All],2,FALSE)</f>
@@ -3344,10 +3344,10 @@
       </c>
       <c r="E73" s="6"/>
       <c r="F73" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="H73" s="1"/>
     </row>
@@ -3356,10 +3356,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C74" s="22" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D74" s="27" t="str">
         <f>VLOOKUP(C74,TablaUnidades[#All],2,FALSE)</f>
@@ -3367,10 +3367,10 @@
       </c>
       <c r="E74" s="6"/>
       <c r="F74" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H74" s="1"/>
     </row>
@@ -3379,10 +3379,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D75" s="27" t="str">
         <f>VLOOKUP(C75,TablaUnidades[#All],2,FALSE)</f>
@@ -3390,10 +3390,10 @@
       </c>
       <c r="E75" s="6"/>
       <c r="F75" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="H75" s="1"/>
     </row>
@@ -3422,7 +3422,7 @@
         <v>133</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D77" s="27" t="str">
         <f>VLOOKUP(C77,TablaUnidades[#All],2,FALSE)</f>
@@ -3433,7 +3433,7 @@
         <v>132</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H77" s="1"/>
     </row>
@@ -3445,7 +3445,7 @@
         <v>76</v>
       </c>
       <c r="C78" s="21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D78" s="27" t="str">
         <f>VLOOKUP(C78,TablaUnidades[#All],2,FALSE)</f>
@@ -3453,10 +3453,10 @@
       </c>
       <c r="E78" s="6"/>
       <c r="F78" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G78" s="12" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="H78" s="1"/>
     </row>
@@ -3468,18 +3468,18 @@
         <v>28</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D79" s="27" t="str">
         <f>VLOOKUP(C79,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="E79" s="1"/>
-      <c r="F79" s="1" t="s">
+      <c r="F79" s="12" t="s">
         <v>117</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="H79" s="1"/>
     </row>
@@ -3488,21 +3488,21 @@
         <v>79</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D80" s="27" t="str">
         <f>VLOOKUP(C80,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="E80" s="1"/>
-      <c r="F80" s="1" t="s">
-        <v>165</v>
+      <c r="F80" s="12" t="s">
+        <v>164</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H80" s="1"/>
     </row>
@@ -3514,7 +3514,7 @@
         <v>69</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D81" s="27" t="str">
         <f>VLOOKUP(C81,TablaUnidades[#All],2,FALSE)</f>
@@ -3525,7 +3525,7 @@
         <v>124</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="H81" s="1"/>
     </row>
@@ -3534,21 +3534,21 @@
         <v>81</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D82" s="27" t="str">
         <f>VLOOKUP(C82,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="E82" s="1"/>
-      <c r="F82" s="1" t="s">
-        <v>153</v>
+      <c r="F82" s="12" t="s">
+        <v>152</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="H82" s="1"/>
     </row>
@@ -3560,7 +3560,7 @@
         <v>54</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D83" s="27" t="str">
         <f>VLOOKUP(C83,TablaUnidades[#All],2,FALSE)</f>
@@ -3568,10 +3568,10 @@
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H83" s="1"/>
     </row>
@@ -3583,7 +3583,7 @@
         <v>5</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D84" s="27" t="str">
         <f>VLOOKUP(C84,TablaUnidades[#All],2,FALSE)</f>
@@ -3594,7 +3594,7 @@
         <v>129</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="H84" s="7"/>
     </row>
@@ -3606,7 +3606,7 @@
         <v>15</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D85" s="27" t="str">
         <f>VLOOKUP(C85,TablaUnidades[#All],2,FALSE)</f>
@@ -3617,7 +3617,7 @@
         <v>94</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="H85" s="7"/>
     </row>
@@ -3646,7 +3646,7 @@
         <v>56</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D87" s="27" t="str">
         <f>VLOOKUP(C87,TablaUnidades[#All],2,FALSE)</f>
@@ -3654,7 +3654,7 @@
       </c>
       <c r="E87" s="7"/>
       <c r="F87" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
@@ -3664,10 +3664,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D88" s="27" t="str">
         <f>VLOOKUP(C88,TablaUnidades[#All],2,FALSE)</f>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="E88" s="7"/>
       <c r="F88" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
@@ -3688,7 +3688,7 @@
         <v>25</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D89" s="27" t="str">
         <f>VLOOKUP(C89,TablaUnidades[#All],2,FALSE)</f>
@@ -3709,7 +3709,7 @@
         <v>75</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D90" s="27" t="str">
         <f>VLOOKUP(C90,TablaUnidades[#All],2,FALSE)</f>
@@ -3717,7 +3717,7 @@
       </c>
       <c r="E90" s="7"/>
       <c r="F90" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G90" s="7"/>
       <c r="H90" s="7"/>
@@ -3730,7 +3730,7 @@
         <v>4</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D91" s="27" t="str">
         <f>VLOOKUP(C91,TablaUnidades[#All],2,FALSE)</f>
@@ -3748,17 +3748,17 @@
         <v>91</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D92" s="27" t="str">
         <f>VLOOKUP(C92,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="F92" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
@@ -3769,7 +3769,7 @@
         <v>126</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D93" s="27" t="str">
         <f>VLOOKUP(C93,TablaUnidades[#All],2,FALSE)</f>
@@ -3790,7 +3790,7 @@
         <v>105</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D94" s="27" t="str">
         <f>VLOOKUP(C94,TablaUnidades[#All],2,FALSE)</f>
@@ -3811,7 +3811,7 @@
         <v>42</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D95" s="27" t="str">
         <f>VLOOKUP(C95,TablaUnidades[#All],2,FALSE)</f>
@@ -3832,7 +3832,7 @@
         <v>47</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D96" s="27" t="str">
         <f>VLOOKUP(C96,TablaUnidades[#All],2,FALSE)</f>
@@ -3840,7 +3840,7 @@
       </c>
       <c r="E96" s="7"/>
       <c r="F96" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G96" s="7"/>
       <c r="H96" s="7"/>
@@ -3850,17 +3850,17 @@
         <v>96</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D97" s="27" t="str">
         <f>VLOOKUP(C97,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por metro</v>
       </c>
       <c r="F97" s="24" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
@@ -3871,14 +3871,14 @@
         <v>51</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D98" s="27" t="str">
         <f>VLOOKUP(C98,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por rollo</v>
       </c>
       <c r="F98" s="24" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
@@ -3889,14 +3889,14 @@
         <v>46</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D99" s="27" t="str">
         <f>VLOOKUP(C99,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por rollo</v>
       </c>
       <c r="F99" s="24" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
@@ -3907,7 +3907,7 @@
         <v>24</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D100" s="27" t="str">
         <f>VLOOKUP(C100,TablaUnidades[#All],2,FALSE)</f>
@@ -3915,7 +3915,7 @@
       </c>
       <c r="E100" s="7"/>
       <c r="F100" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G100" s="7"/>
       <c r="H100" s="7"/>
@@ -3925,17 +3925,17 @@
         <v>100</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D101" s="27" t="str">
         <f>VLOOKUP(C101,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="F101" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
@@ -3946,7 +3946,7 @@
         <v>140</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D102" s="27" t="str">
         <f>VLOOKUP(C102,TablaUnidades[#All],2,FALSE)</f>
@@ -3967,7 +3967,7 @@
         <v>142</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D103" s="27" t="str">
         <f>VLOOKUP(C103,TablaUnidades[#All],2,FALSE)</f>
@@ -3988,7 +3988,7 @@
         <v>92</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D104" s="27" t="str">
         <f>VLOOKUP(C104,TablaUnidades[#All],2,FALSE)</f>
@@ -4009,7 +4009,7 @@
         <v>21</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D105" s="27" t="str">
         <f>VLOOKUP(C105,TablaUnidades[#All],2,FALSE)</f>
@@ -4027,17 +4027,17 @@
         <v>105</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D106" s="27" t="str">
         <f>VLOOKUP(C106,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="F106" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
@@ -4048,7 +4048,7 @@
         <v>20</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D107" s="27" t="str">
         <f>VLOOKUP(C107,TablaUnidades[#All],2,FALSE)</f>
@@ -4069,14 +4069,14 @@
         <v>62</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D108" s="27" t="str">
         <f>VLOOKUP(C108,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="F108" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
@@ -4084,17 +4084,17 @@
         <v>108</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D109" s="27" t="str">
         <f>VLOOKUP(C109,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="F109" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
@@ -4105,7 +4105,7 @@
         <v>34</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D110" s="27" t="str">
         <f>VLOOKUP(C110,TablaUnidades[#All],2,FALSE)</f>
@@ -4126,14 +4126,14 @@
         <v>53</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D111" s="27" t="str">
         <f>VLOOKUP(C111,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="F111" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
@@ -4144,7 +4144,7 @@
         <v>10</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D112" s="27" t="str">
         <f>VLOOKUP(C112,TablaUnidades[#All],2,FALSE)</f>
@@ -4165,7 +4165,7 @@
         <v>36</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D113" s="27" t="str">
         <f>VLOOKUP(C113,TablaUnidades[#All],2,FALSE)</f>
@@ -4186,7 +4186,7 @@
         <v>37</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D114" s="27" t="str">
         <f>VLOOKUP(C114,TablaUnidades[#All],2,FALSE)</f>
@@ -4204,17 +4204,17 @@
         <v>114</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D115" s="27" t="str">
         <f>VLOOKUP(C115,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="F115" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
@@ -4239,17 +4239,17 @@
         <v>116</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C117" s="23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D117" s="27" t="str">
         <f>VLOOKUP(C117,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="F117" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
@@ -4277,14 +4277,14 @@
         <v>65</v>
       </c>
       <c r="C119" s="23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D119" s="27" t="str">
         <f>VLOOKUP(C119,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="F119" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
@@ -4295,7 +4295,7 @@
         <v>41</v>
       </c>
       <c r="C120" s="23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D120" s="27" t="str">
         <f>VLOOKUP(C120,TablaUnidades[#All],2,FALSE)</f>
@@ -4303,7 +4303,7 @@
       </c>
       <c r="E120" s="7"/>
       <c r="F120" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G120" s="7"/>
       <c r="H120" s="7"/>
@@ -4333,7 +4333,7 @@
         <v>123</v>
       </c>
       <c r="C122" s="23" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D122" s="27" t="str">
         <f>VLOOKUP(C122,TablaUnidades[#All],2,FALSE)</f>
@@ -4354,7 +4354,7 @@
         <v>16</v>
       </c>
       <c r="C123" s="23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D123" s="27" t="str">
         <f>VLOOKUP(C123,TablaUnidades[#All],2,FALSE)</f>
@@ -4375,7 +4375,7 @@
         <v>52</v>
       </c>
       <c r="C124" s="23" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D124" s="27" t="str">
         <f>VLOOKUP(C124,TablaUnidades[#All],2,FALSE)</f>
@@ -4383,7 +4383,7 @@
       </c>
       <c r="E124" s="7"/>
       <c r="F124" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G124" s="7"/>
       <c r="H124" s="7"/>
@@ -4396,7 +4396,7 @@
         <v>115</v>
       </c>
       <c r="C125" s="23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D125" s="27" t="str">
         <f>VLOOKUP(C125,TablaUnidades[#All],2,FALSE)</f>
@@ -4414,17 +4414,17 @@
         <v>125</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C126" s="23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D126" s="27" t="str">
         <f>VLOOKUP(C126,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="F126" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
@@ -4435,14 +4435,14 @@
         <v>58</v>
       </c>
       <c r="C127" s="23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D127" s="27" t="str">
         <f>VLOOKUP(C127,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="F127" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
@@ -4453,7 +4453,7 @@
         <v>23</v>
       </c>
       <c r="C128" s="23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D128" s="27" t="str">
         <f>VLOOKUP(C128,TablaUnidades[#All],2,FALSE)</f>
@@ -4474,14 +4474,14 @@
         <v>57</v>
       </c>
       <c r="C129" s="23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D129" s="27" t="str">
         <f>VLOOKUP(C129,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="F129" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
@@ -4492,11 +4492,11 @@
         <v>6</v>
       </c>
       <c r="C130" s="23" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="D130" s="27" t="str">
         <f>VLOOKUP(C130,TablaUnidades[#All],2,FALSE)</f>
-        <v>precio por botella</v>
+        <v>precio por litro</v>
       </c>
       <c r="E130" s="7"/>
       <c r="F130" s="17" t="s">
@@ -4513,7 +4513,7 @@
         <v>7</v>
       </c>
       <c r="C131" s="23" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D131" s="27" t="str">
         <f>VLOOKUP(C131,TablaUnidades[#All],2,FALSE)</f>
@@ -4534,7 +4534,7 @@
         <v>70</v>
       </c>
       <c r="C132" s="23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D132" s="27" t="str">
         <f>VLOOKUP(C132,TablaUnidades[#All],2,FALSE)</f>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="E132" s="7"/>
       <c r="F132" s="17" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G132" s="7"/>
       <c r="H132" s="7"/>
@@ -4555,14 +4555,14 @@
         <v>66</v>
       </c>
       <c r="C133" s="23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D133" s="27" t="str">
         <f>VLOOKUP(C133,TablaUnidades[#All],2,FALSE)</f>
         <v>precio por kilo</v>
       </c>
       <c r="F133" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
@@ -4570,7 +4570,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="14" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C134" s="23"/>
       <c r="D134" s="27" t="e">
@@ -4583,17 +4583,17 @@
         <v>134</v>
       </c>
       <c r="B135" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C135" s="23" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D135" s="27" t="str">
         <f>VLOOKUP(C135,TablaUnidades[#All],2,FALSE)</f>
         <v>Comprueba que la unidad son 100 ML</v>
       </c>
       <c r="F135" s="24" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -4643,9 +4643,22 @@
     <hyperlink ref="F122" r:id="rId35" xr:uid="{6C04EF90-3ED9-4148-9AB7-1555F2F7C0DB}"/>
     <hyperlink ref="F132" r:id="rId36" xr:uid="{BCC38D84-87A8-43DC-B02E-BFDF89E23C40}"/>
     <hyperlink ref="F135" r:id="rId37" xr:uid="{E1BFAD03-ACD1-4E65-94B5-4BD5A7F13029}"/>
+    <hyperlink ref="F38" r:id="rId38" xr:uid="{FE74EC56-25E2-443A-820F-F8A329D059AF}"/>
+    <hyperlink ref="G38" r:id="rId39" xr:uid="{33C935BA-D7FD-4588-B488-205019CB622D}"/>
+    <hyperlink ref="F60" r:id="rId40" xr:uid="{4A424611-A6E9-41A9-AEAE-7DFEA64606C7}"/>
+    <hyperlink ref="G60" r:id="rId41" xr:uid="{A233FE08-D6FF-468B-91F3-9EFE2DD83CB9}"/>
+    <hyperlink ref="F82" r:id="rId42" xr:uid="{060A0BCD-8D30-438C-AB40-FEFDF4DE4288}"/>
+    <hyperlink ref="F79" r:id="rId43" xr:uid="{DB9D786E-0C2D-43B5-B54C-1588832C927D}"/>
+    <hyperlink ref="F80" r:id="rId44" xr:uid="{41DD9D17-B29C-480A-B66B-9686593DCAE5}"/>
+    <hyperlink ref="F30" r:id="rId45" xr:uid="{6AC629B3-C7AA-463D-A5E0-5E0BDA3DF810}"/>
+    <hyperlink ref="G30" r:id="rId46" xr:uid="{762FDD71-4AB6-4935-80AB-40BC37B09712}"/>
+    <hyperlink ref="F42" r:id="rId47" xr:uid="{21D809AC-7F12-4D55-A714-4F5842994E1F}"/>
+    <hyperlink ref="F3" r:id="rId48" xr:uid="{2590EA00-331B-486E-AA14-DC5BC463C185}"/>
+    <hyperlink ref="G3" r:id="rId49" xr:uid="{F0195699-F598-41E1-9EEB-254D72337106}"/>
+    <hyperlink ref="G4" r:id="rId50" xr:uid="{CA071640-A5CC-4E59-B038-F4016F0476DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId51"/>
 </worksheet>
 </file>
 
@@ -4664,90 +4677,90 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>